<commit_message>
Add rounding to line 6 of child tax worksheet
</commit_message>
<xml_diff>
--- a/Federal/f1040-combined-2019.xlsx
+++ b/Federal/f1040-combined-2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IRS f1040" sheetId="1" state="visible" r:id="rId2"/>
@@ -1061,13 +1061,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1108,17 +1107,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1359,13 +1348,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="91">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1466,35 +1455,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1502,7 +1483,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1514,11 +1495,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1558,7 +1539,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1686,7 +1667,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1694,15 +1675,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="17" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2572,6 +2553,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2585,216 +2567,216 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="2" t="s">
         <v>90</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="29" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="29" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="36"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="str">
+      <c r="A21" s="28" t="str">
         <f aca="false">"13."</f>
         <v>13.</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="29" t="str">
+      <c r="B21" s="29"/>
+      <c r="C21" s="2" t="str">
         <f aca="false">"13."</f>
         <v>13.</v>
       </c>
@@ -2802,91 +2784,91 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="2" t="s">
         <v>111</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="36"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="2" t="s">
         <v>121</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="2" t="s">
         <v>123</v>
       </c>
       <c r="D28" s="4"/>
@@ -2944,7 +2926,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,21 +2948,21 @@
       <c r="D2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="39" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="41"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2986,27 +2970,27 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>130</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -3014,13 +2998,13 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>132</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3028,13 +3012,13 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>134</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -3042,13 +3026,13 @@
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3056,13 +3040,13 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>137</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -3070,38 +3054,38 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="37" t="s">
         <v>139</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="39" t="s">
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="39" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="41" t="n">
+      <c r="F12" s="39" t="n">
         <f aca="false">SUM(F3:F11)</f>
         <v>0</v>
       </c>
@@ -3115,21 +3099,21 @@
       <c r="D13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="39" t="s">
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="41"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>144</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -3137,13 +3121,13 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="F15" s="41"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>146</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -3151,13 +3135,13 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="41"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -3165,13 +3149,13 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="39"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -3179,13 +3163,13 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3193,13 +3177,13 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3207,13 +3191,13 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -3221,13 +3205,13 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="41"/>
+      <c r="F21" s="39"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="37" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -3235,41 +3219,41 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="39"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="37" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -3277,13 +3261,13 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="41"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="37" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -3291,13 +3275,13 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="37" t="s">
         <v>158</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3305,24 +3289,24 @@
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="39" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="41" t="n">
+      <c r="F28" s="39" t="n">
         <f aca="false">SUM(F14:F27)</f>
         <v>0</v>
       </c>
@@ -3380,7 +3364,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,46 +3388,46 @@
       <c r="D3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="48"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="39" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="39" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="48" t="n">
+      <c r="F6" s="46" t="n">
         <f aca="false">SUM(F4:F5)</f>
         <v>0</v>
       </c>
@@ -3455,116 +3441,116 @@
       <c r="D8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="39" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="48"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="39" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="48"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="39" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="39" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="48"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="39" t="s">
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="48"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="39" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F14" s="48"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="51"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="39" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="48" t="n">
+      <c r="F16" s="46" t="n">
         <f aca="false">SUM(F9:F14)</f>
         <v>0</v>
       </c>
@@ -3611,15 +3597,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
@@ -3630,88 +3617,88 @@
       <c r="D2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="46"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="46"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="46"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="48" t="n">
+      <c r="D9" s="46" t="n">
         <f aca="false">SUM(D3:D8)</f>
         <v>0</v>
       </c>
@@ -3725,88 +3712,88 @@
       <c r="D11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="48"/>
+      <c r="D13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="46"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="46"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="46"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="48" t="n">
+      <c r="D18" s="46" t="n">
         <f aca="false">SUM(D12:D17)</f>
         <v>0</v>
       </c>
@@ -3834,16 +3821,18 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,241 +3844,241 @@
       <c r="D1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="55" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="39" t="s">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="48" t="n">
+      <c r="F6" s="46" t="n">
         <f aca="false">D5*2000</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="39" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="48" t="n">
+      <c r="F8" s="46" t="n">
         <f aca="false">D7*500</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="39" t="s">
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="48" t="n">
+      <c r="F9" s="46" t="n">
         <f aca="false">F6+F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="48" t="n">
+      <c r="D10" s="46" t="n">
         <f aca="false">'IRS f1040'!F17</f>
         <v>0</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63"/>
-      <c r="B12" s="60" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="63"/>
-      <c r="B13" s="60" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="48" t="n">
-        <f aca="false">IF(D10&gt;D11,D10-D11,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
+      <c r="D14" s="46" t="n">
+        <f aca="false">ROUNDUP(IF(D10&gt;D11,D10-D11,0),-3)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="63"/>
-      <c r="B15" s="60" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="63"/>
-      <c r="B16" s="60" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="63"/>
-      <c r="B17" s="60" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="62"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="39" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="F18" s="48" t="n">
+      <c r="F18" s="46" t="n">
         <f aca="false">D14*0.05</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="39" t="s">
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F19" s="48" t="n">
+      <c r="F19" s="46" t="n">
         <f aca="false">IF(F9&gt;F18,F9-F18,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="64"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
@@ -4100,220 +4089,220 @@
       <c r="D23" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="55" t="s">
         <v>215</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="39" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="48" t="n">
+      <c r="F25" s="46" t="n">
         <f aca="false">'IRS f1040'!F28</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="62"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="63"/>
-      <c r="B27" s="60" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="58" t="s">
         <v>217</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="48" t="n">
+      <c r="C27" s="58"/>
+      <c r="D27" s="46" t="n">
         <f aca="false">'IRS f1040 Schedule 3'!D3</f>
         <v>0</v>
       </c>
-      <c r="E27" s="61"/>
-      <c r="F27" s="62"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="63"/>
-      <c r="B28" s="60" t="s">
+      <c r="A28" s="61"/>
+      <c r="B28" s="58" t="s">
         <v>218</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="48" t="n">
+      <c r="C28" s="58"/>
+      <c r="D28" s="46" t="n">
         <f aca="false">'IRS f1040 Schedule 3'!D4</f>
         <v>0</v>
       </c>
-      <c r="E28" s="61"/>
-      <c r="F28" s="62"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="63"/>
-      <c r="B29" s="60" t="s">
+      <c r="A29" s="61"/>
+      <c r="B29" s="58" t="s">
         <v>219</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="48" t="n">
+      <c r="C29" s="58"/>
+      <c r="D29" s="46" t="n">
         <f aca="false">'IRS f1040 Schedule 3'!D5</f>
         <v>0</v>
       </c>
-      <c r="E29" s="61"/>
-      <c r="F29" s="62"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="63"/>
-      <c r="B30" s="60" t="s">
+      <c r="A30" s="61"/>
+      <c r="B30" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="62"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="63"/>
-      <c r="B31" s="60" t="s">
+      <c r="A31" s="61"/>
+      <c r="B31" s="58" t="s">
         <v>221</v>
       </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="62"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="63"/>
-      <c r="B32" s="60" t="s">
+      <c r="A32" s="61"/>
+      <c r="B32" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="60"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="63"/>
-      <c r="B33" s="60" t="s">
+      <c r="A33" s="61"/>
+      <c r="B33" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="62"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="63"/>
-      <c r="B34" s="60" t="s">
+      <c r="A34" s="61"/>
+      <c r="B34" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="62"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="39" t="s">
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="48" t="n">
+      <c r="F35" s="46" t="n">
         <f aca="false">SUM(D27:D34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="63"/>
-      <c r="B36" s="60" t="s">
+      <c r="A36" s="61"/>
+      <c r="B36" s="58" t="s">
         <v>226</v>
       </c>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="68"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="66"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="63"/>
-      <c r="B37" s="60" t="s">
+      <c r="A37" s="61"/>
+      <c r="B37" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="68"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="66"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="39" t="s">
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="F38" s="48" t="n">
+      <c r="F38" s="46" t="n">
         <f aca="false">F25-F35</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="69"/>
-      <c r="B39" s="60" t="s">
+      <c r="A39" s="67"/>
+      <c r="B39" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="68"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="66"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="69"/>
-      <c r="B40" s="60" t="s">
+      <c r="A40" s="67"/>
+      <c r="B40" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="68"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="66"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="69"/>
-      <c r="B41" s="60" t="s">
+      <c r="A41" s="67"/>
+      <c r="B41" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="68"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="66"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="39" t="s">
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="F42" s="48" t="n">
+      <c r="F42" s="46" t="n">
         <f aca="false">IF(F19&gt;F38,F38,F19)</f>
         <v>0</v>
       </c>
@@ -4351,7 +4340,7 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -4366,14 +4355,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
@@ -4384,450 +4373,450 @@
       <c r="D2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="68" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="72"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="71" t="s">
         <v>237</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="74"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="71" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="74"/>
-    </row>
-    <row r="8" s="77" customFormat="true" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="73" t="s">
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="72"/>
+    </row>
+    <row r="8" s="75" customFormat="true" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="71" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="74"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="74"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="78"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="74"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="39" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="48" t="n">
+      <c r="F12" s="46" t="n">
         <f aca="false">'IRS f1040 Child Tax Credit'!F19</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="79" t="s">
         <v>242</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="39" t="s">
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="82" t="n">
+      <c r="F13" s="80" t="n">
         <f aca="false">'IRS f1040'!D29</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="79" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="39" t="s">
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="48" t="n">
+      <c r="F14" s="46" t="n">
         <f aca="false">F12-F13</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="79" t="s">
         <v>244</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="39" t="s">
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="42"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="79" t="s">
         <v>245</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="39" t="s">
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="48" t="n">
+      <c r="F16" s="46" t="n">
         <f aca="false">F15*1400</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="39" t="s">
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="48" t="n">
+      <c r="F17" s="46" t="n">
         <f aca="false">F15*1400</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="71" t="s">
         <v>246</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="72"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="79" t="s">
         <v>247</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="39" t="s">
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="83" t="n">
+      <c r="F19" s="81" t="n">
         <f aca="false">MIN(F14,F17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="73" t="s">
         <v>249</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="D20" s="84"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="74"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="72"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="73" t="s">
         <v>251</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="D21" s="84"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="74"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="72"/>
     </row>
     <row r="22" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="84" t="n">
+      <c r="D22" s="82" t="n">
         <f aca="false">IF(D20&gt;2500,D20-2500,0)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="54"/>
-      <c r="F22" s="74"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="72"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="79" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="39" t="s">
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="48" t="n">
+      <c r="F23" s="46" t="n">
         <f aca="false">D22*0.15</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="74"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="72"/>
     </row>
     <row r="25" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="79" t="s">
         <v>255</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="39" t="s">
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="41" t="n">
+      <c r="F25" s="39" t="n">
         <f aca="false">IF(F23=0,0,MIN(F19,F23))</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="39" t="s">
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="83" t="n">
+      <c r="F26" s="81" t="n">
         <f aca="false">IF(F23&gt;=F19,F19,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="86" t="s">
+      <c r="A27" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
     </row>
     <row r="28" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="85" t="s">
         <v>258</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="88" t="n">
+      <c r="D28" s="86" t="n">
         <f aca="false">W2!D9+W2!D11</f>
         <v>0</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="72"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="70"/>
     </row>
     <row r="29" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="73" t="s">
         <v>259</v>
       </c>
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="88" t="n">
+      <c r="D29" s="86" t="n">
         <f aca="false">'IRS f1040 Schedule 1'!F18+'IRS f1040 Schedule 2'!F10+'IRS f1040 Schedule 2'!F14</f>
         <v>0</v>
       </c>
-      <c r="E29" s="54"/>
-      <c r="F29" s="74"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="72"/>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="79" t="s">
+      <c r="C30" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="88" t="n">
+      <c r="D30" s="86" t="n">
         <f aca="false">D28+D29</f>
         <v>0</v>
       </c>
-      <c r="E30" s="54"/>
-      <c r="F30" s="74"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="72"/>
     </row>
     <row r="31" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="D31" s="88" t="n">
+      <c r="D31" s="86" t="n">
         <f aca="false">'IRS f1040'!D35+'IRS f1040 Schedule 3'!D15</f>
         <v>0</v>
       </c>
-      <c r="E31" s="54"/>
-      <c r="F31" s="74"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="72"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="79" t="s">
         <v>261</v>
       </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="39" t="s">
+      <c r="C32" s="79"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="F32" s="41" t="n">
+      <c r="F32" s="39" t="n">
         <f aca="false">D30-D31</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="79" t="s">
         <v>262</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="39" t="s">
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="41" t="n">
+      <c r="F33" s="39" t="n">
         <f aca="false">MAX(F32,F23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="89"/>
-      <c r="B34" s="85" t="s">
+      <c r="A34" s="87"/>
+      <c r="B34" s="83" t="s">
         <v>263</v>
       </c>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="90"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="88"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="89" t="s">
         <v>264</v>
       </c>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="92" t="s">
+      <c r="B36" s="90" t="s">
         <v>265</v>
       </c>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="39" t="s">
+      <c r="C36" s="90"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="41" t="n">
+      <c r="F36" s="39" t="n">
         <f aca="false">MIN(F33,F19)</f>
         <v>0</v>
       </c>

</xml_diff>